<commit_message>
richards: newton cooling test created and doco updated
r23680
</commit_message>
<xml_diff>
--- a/modules/combined/doc/richards/tests/data/nc.xlsx
+++ b/modules/combined/doc/richards/tests/data/nc.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="nc01" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="L:\moose\trunk\wallaby\doc\tests\data\nc01.csv" comma="1">
+    <textPr codePage="850" sourceFile="L:\moose\project2\trunk\elk\doc\richards\tests\data\nc01.csv" comma="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -39,7 +39,7 @@
     </textPr>
   </connection>
   <connection id="2" name="nc01_analytic" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="L:\moose\trunk\wallaby\doc\tests\data\nc01_analytic.txt">
+    <textPr codePage="850" sourceFile="L:\moose\project2\trunk\elk\doc\richards\tests\data\nc01_analytic.txt">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -60,7 +60,7 @@
     </textPr>
   </connection>
   <connection id="4" name="nc02_analytic" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="L:\moose\trunk\wallaby\doc\tests\data\nc02_analytic.txt">
+    <textPr codePage="850" sourceFile="L:\moose\project2\trunk\elk\doc\richards\tests\data\nc02_analytic.txt">
       <textFields>
         <textField/>
       </textFields>
@@ -1157,10 +1157,10 @@
                   <c:v>1990900</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1989500</c:v>
+                  <c:v>1989600</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1988100</c:v>
+                  <c:v>1988200</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1986700</c:v>
@@ -1175,19 +1175,19 @@
                   <c:v>1982200</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1980600</c:v>
+                  <c:v>1980700</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1979000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1977300</c:v>
+                  <c:v>1977400</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1975600</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1973800</c:v>
+                  <c:v>1973900</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1972000</c:v>
@@ -1217,10 +1217,10 @@
                   <c:v>1954500</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1951900</c:v>
+                  <c:v>1952000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1949200</c:v>
+                  <c:v>1949300</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>1946500</c:v>
@@ -1232,184 +1232,184 @@
                   <c:v>1940600</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1937400</c:v>
+                  <c:v>1937500</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>1934200</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1930800</c:v>
+                  <c:v>1930900</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1927300</c:v>
+                  <c:v>1927400</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1923600</c:v>
+                  <c:v>1923700</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>1919900</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1915900</c:v>
+                  <c:v>1916000</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1911800</c:v>
+                  <c:v>1911900</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>1907600</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1903100</c:v>
+                  <c:v>1903200</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>1898600</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1893800</c:v>
+                  <c:v>1893900</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1888800</c:v>
+                  <c:v>1888900</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1883700</c:v>
+                  <c:v>1883800</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1878400</c:v>
+                  <c:v>1878500</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1872900</c:v>
+                  <c:v>1873000</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1867100</c:v>
+                  <c:v>1867200</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1861200</c:v>
+                  <c:v>1861300</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1855000</c:v>
+                  <c:v>1855100</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1848600</c:v>
+                  <c:v>1848700</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1842000</c:v>
+                  <c:v>1842100</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1835100</c:v>
+                  <c:v>1835300</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1828000</c:v>
+                  <c:v>1828200</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1820700</c:v>
+                  <c:v>1820800</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1813000</c:v>
+                  <c:v>1813200</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1805100</c:v>
+                  <c:v>1805300</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1796900</c:v>
+                  <c:v>1797100</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1788500</c:v>
+                  <c:v>1788600</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1779700</c:v>
+                  <c:v>1779800</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1770600</c:v>
+                  <c:v>1770800</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1761200</c:v>
+                  <c:v>1761400</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1751500</c:v>
+                  <c:v>1751700</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1741500</c:v>
+                  <c:v>1741600</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1731100</c:v>
+                  <c:v>1731200</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1720300</c:v>
+                  <c:v>1720500</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1709200</c:v>
+                  <c:v>1709400</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1697700</c:v>
+                  <c:v>1697900</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1685800</c:v>
+                  <c:v>1686000</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1673500</c:v>
+                  <c:v>1673700</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1660800</c:v>
+                  <c:v>1661000</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1647600</c:v>
+                  <c:v>1647800</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1634000</c:v>
+                  <c:v>1634200</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1620000</c:v>
+                  <c:v>1620200</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1605500</c:v>
+                  <c:v>1605700</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1590500</c:v>
+                  <c:v>1590600</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1574900</c:v>
+                  <c:v>1575100</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1558900</c:v>
+                  <c:v>1559100</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1542300</c:v>
+                  <c:v>1542500</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1525100</c:v>
+                  <c:v>1525300</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1507400</c:v>
+                  <c:v>1507500</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1489000</c:v>
+                  <c:v>1489200</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1470000</c:v>
+                  <c:v>1470200</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1450400</c:v>
+                  <c:v>1450500</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1430000</c:v>
+                  <c:v>1430200</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1409000</c:v>
+                  <c:v>1409100</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1387200</c:v>
+                  <c:v>1387300</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1364600</c:v>
+                  <c:v>1364700</c:v>
                 </c:pt>
                 <c:pt idx="90">
                   <c:v>1341200</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1316900</c:v>
+                  <c:v>1317000</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1291700</c:v>
+                  <c:v>1291800</c:v>
                 </c:pt>
                 <c:pt idx="93">
                   <c:v>1265700</c:v>
@@ -1421,19 +1421,19 @@
                   <c:v>1210400</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1181200</c:v>
+                  <c:v>1181100</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1150800</c:v>
+                  <c:v>1150700</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1119200</c:v>
+                  <c:v>1119000</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1086200</c:v>
+                  <c:v>1086000</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1051900</c:v>
+                  <c:v>1051600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2719,11 +2719,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="151428480"/>
-        <c:axId val="128615552"/>
+        <c:axId val="96050176"/>
+        <c:axId val="103200256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="151428480"/>
+        <c:axId val="96050176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2749,12 +2749,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128615552"/>
+        <c:crossAx val="103200256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="128615552"/>
+        <c:axId val="103200256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000000"/>
@@ -2787,7 +2787,7 @@
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151428480"/>
+        <c:crossAx val="96050176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2805,7 +2805,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3364,7 +3364,7 @@
     </row>
     <row r="12" spans="3:9">
       <c r="C12" s="1">
-        <v>1989500</v>
+        <v>1989600</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="13" spans="3:9">
       <c r="C13" s="1">
-        <v>1988100</v>
+        <v>1988200</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -3502,7 +3502,7 @@
     </row>
     <row r="18" spans="3:9">
       <c r="C18" s="1">
-        <v>1980600</v>
+        <v>1980700</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -3548,7 +3548,7 @@
     </row>
     <row r="20" spans="3:9">
       <c r="C20" s="1">
-        <v>1977300</v>
+        <v>1977400</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -3594,7 +3594,7 @@
     </row>
     <row r="22" spans="3:9">
       <c r="C22" s="1">
-        <v>1973800</v>
+        <v>1973900</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -3824,7 +3824,7 @@
     </row>
     <row r="32" spans="3:9">
       <c r="C32" s="1">
-        <v>1951900</v>
+        <v>1952000</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -3847,7 +3847,7 @@
     </row>
     <row r="33" spans="3:9">
       <c r="C33" s="1">
-        <v>1949200</v>
+        <v>1949300</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -3939,7 +3939,7 @@
     </row>
     <row r="37" spans="3:9">
       <c r="C37" s="1">
-        <v>1937400</v>
+        <v>1937500</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -3985,7 +3985,7 @@
     </row>
     <row r="39" spans="3:9">
       <c r="C39" s="1">
-        <v>1930800</v>
+        <v>1930900</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -4008,7 +4008,7 @@
     </row>
     <row r="40" spans="3:9">
       <c r="C40" s="1">
-        <v>1927300</v>
+        <v>1927400</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -4031,7 +4031,7 @@
     </row>
     <row r="41" spans="3:9">
       <c r="C41" s="1">
-        <v>1923600</v>
+        <v>1923700</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -4077,7 +4077,7 @@
     </row>
     <row r="43" spans="3:9">
       <c r="C43" s="1">
-        <v>1915900</v>
+        <v>1916000</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -4100,7 +4100,7 @@
     </row>
     <row r="44" spans="3:9">
       <c r="C44" s="1">
-        <v>1911800</v>
+        <v>1911900</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -4146,7 +4146,7 @@
     </row>
     <row r="46" spans="3:9">
       <c r="C46" s="1">
-        <v>1903100</v>
+        <v>1903200</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -4192,7 +4192,7 @@
     </row>
     <row r="48" spans="3:9">
       <c r="C48" s="1">
-        <v>1893800</v>
+        <v>1893900</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -4215,7 +4215,7 @@
     </row>
     <row r="49" spans="3:9">
       <c r="C49" s="1">
-        <v>1888800</v>
+        <v>1888900</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -4238,7 +4238,7 @@
     </row>
     <row r="50" spans="3:9">
       <c r="C50" s="1">
-        <v>1883700</v>
+        <v>1883800</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -4261,7 +4261,7 @@
     </row>
     <row r="51" spans="3:9">
       <c r="C51" s="1">
-        <v>1878400</v>
+        <v>1878500</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -4284,7 +4284,7 @@
     </row>
     <row r="52" spans="3:9">
       <c r="C52" s="1">
-        <v>1872900</v>
+        <v>1873000</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -4307,7 +4307,7 @@
     </row>
     <row r="53" spans="3:9">
       <c r="C53" s="1">
-        <v>1867100</v>
+        <v>1867200</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -4330,7 +4330,7 @@
     </row>
     <row r="54" spans="3:9">
       <c r="C54" s="1">
-        <v>1861200</v>
+        <v>1861300</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -4353,7 +4353,7 @@
     </row>
     <row r="55" spans="3:9">
       <c r="C55" s="1">
-        <v>1855000</v>
+        <v>1855100</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -4376,7 +4376,7 @@
     </row>
     <row r="56" spans="3:9">
       <c r="C56" s="1">
-        <v>1848600</v>
+        <v>1848700</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -4399,7 +4399,7 @@
     </row>
     <row r="57" spans="3:9">
       <c r="C57" s="1">
-        <v>1842000</v>
+        <v>1842100</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -4422,7 +4422,7 @@
     </row>
     <row r="58" spans="3:9">
       <c r="C58" s="1">
-        <v>1835100</v>
+        <v>1835300</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -4445,7 +4445,7 @@
     </row>
     <row r="59" spans="3:9">
       <c r="C59" s="1">
-        <v>1828000</v>
+        <v>1828200</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -4468,7 +4468,7 @@
     </row>
     <row r="60" spans="3:9">
       <c r="C60" s="1">
-        <v>1820700</v>
+        <v>1820800</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -4491,7 +4491,7 @@
     </row>
     <row r="61" spans="3:9">
       <c r="C61" s="1">
-        <v>1813000</v>
+        <v>1813200</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -4514,7 +4514,7 @@
     </row>
     <row r="62" spans="3:9">
       <c r="C62" s="1">
-        <v>1805100</v>
+        <v>1805300</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -4537,7 +4537,7 @@
     </row>
     <row r="63" spans="3:9">
       <c r="C63" s="1">
-        <v>1796900</v>
+        <v>1797100</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -4560,7 +4560,7 @@
     </row>
     <row r="64" spans="3:9">
       <c r="C64" s="1">
-        <v>1788500</v>
+        <v>1788600</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -4583,7 +4583,7 @@
     </row>
     <row r="65" spans="3:9">
       <c r="C65" s="1">
-        <v>1779700</v>
+        <v>1779800</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -4606,7 +4606,7 @@
     </row>
     <row r="66" spans="3:9">
       <c r="C66" s="1">
-        <v>1770600</v>
+        <v>1770800</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -4629,7 +4629,7 @@
     </row>
     <row r="67" spans="3:9">
       <c r="C67" s="1">
-        <v>1761200</v>
+        <v>1761400</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -4652,7 +4652,7 @@
     </row>
     <row r="68" spans="3:9">
       <c r="C68" s="1">
-        <v>1751500</v>
+        <v>1751700</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -4675,7 +4675,7 @@
     </row>
     <row r="69" spans="3:9">
       <c r="C69" s="1">
-        <v>1741500</v>
+        <v>1741600</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -4698,7 +4698,7 @@
     </row>
     <row r="70" spans="3:9">
       <c r="C70" s="1">
-        <v>1731100</v>
+        <v>1731200</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -4721,7 +4721,7 @@
     </row>
     <row r="71" spans="3:9">
       <c r="C71" s="1">
-        <v>1720300</v>
+        <v>1720500</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -4744,7 +4744,7 @@
     </row>
     <row r="72" spans="3:9">
       <c r="C72" s="1">
-        <v>1709200</v>
+        <v>1709400</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -4767,7 +4767,7 @@
     </row>
     <row r="73" spans="3:9">
       <c r="C73" s="1">
-        <v>1697700</v>
+        <v>1697900</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -4790,7 +4790,7 @@
     </row>
     <row r="74" spans="3:9">
       <c r="C74" s="1">
-        <v>1685800</v>
+        <v>1686000</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -4813,7 +4813,7 @@
     </row>
     <row r="75" spans="3:9">
       <c r="C75" s="1">
-        <v>1673500</v>
+        <v>1673700</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -4836,7 +4836,7 @@
     </row>
     <row r="76" spans="3:9">
       <c r="C76" s="1">
-        <v>1660800</v>
+        <v>1661000</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -4859,7 +4859,7 @@
     </row>
     <row r="77" spans="3:9">
       <c r="C77" s="1">
-        <v>1647600</v>
+        <v>1647800</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -4882,7 +4882,7 @@
     </row>
     <row r="78" spans="3:9">
       <c r="C78" s="1">
-        <v>1634000</v>
+        <v>1634200</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -4905,7 +4905,7 @@
     </row>
     <row r="79" spans="3:9">
       <c r="C79" s="1">
-        <v>1620000</v>
+        <v>1620200</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -4928,7 +4928,7 @@
     </row>
     <row r="80" spans="3:9">
       <c r="C80" s="1">
-        <v>1605500</v>
+        <v>1605700</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -4951,7 +4951,7 @@
     </row>
     <row r="81" spans="3:9">
       <c r="C81" s="1">
-        <v>1590500</v>
+        <v>1590600</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -4974,7 +4974,7 @@
     </row>
     <row r="82" spans="3:9">
       <c r="C82" s="1">
-        <v>1574900</v>
+        <v>1575100</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -4997,7 +4997,7 @@
     </row>
     <row r="83" spans="3:9">
       <c r="C83" s="1">
-        <v>1558900</v>
+        <v>1559100</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -5020,7 +5020,7 @@
     </row>
     <row r="84" spans="3:9">
       <c r="C84" s="1">
-        <v>1542300</v>
+        <v>1542500</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -5043,7 +5043,7 @@
     </row>
     <row r="85" spans="3:9">
       <c r="C85" s="1">
-        <v>1525100</v>
+        <v>1525300</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -5066,7 +5066,7 @@
     </row>
     <row r="86" spans="3:9">
       <c r="C86" s="1">
-        <v>1507400</v>
+        <v>1507500</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -5089,7 +5089,7 @@
     </row>
     <row r="87" spans="3:9">
       <c r="C87" s="1">
-        <v>1489000</v>
+        <v>1489200</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -5112,7 +5112,7 @@
     </row>
     <row r="88" spans="3:9">
       <c r="C88" s="1">
-        <v>1470000</v>
+        <v>1470200</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -5135,7 +5135,7 @@
     </row>
     <row r="89" spans="3:9">
       <c r="C89" s="1">
-        <v>1450400</v>
+        <v>1450500</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -5158,7 +5158,7 @@
     </row>
     <row r="90" spans="3:9">
       <c r="C90" s="1">
-        <v>1430000</v>
+        <v>1430200</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -5181,7 +5181,7 @@
     </row>
     <row r="91" spans="3:9">
       <c r="C91" s="1">
-        <v>1409000</v>
+        <v>1409100</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -5204,7 +5204,7 @@
     </row>
     <row r="92" spans="3:9">
       <c r="C92" s="1">
-        <v>1387200</v>
+        <v>1387300</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -5227,7 +5227,7 @@
     </row>
     <row r="93" spans="3:9">
       <c r="C93" s="1">
-        <v>1364600</v>
+        <v>1364700</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -5273,7 +5273,7 @@
     </row>
     <row r="95" spans="3:9">
       <c r="C95" s="1">
-        <v>1316900</v>
+        <v>1317000</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -5296,7 +5296,7 @@
     </row>
     <row r="96" spans="3:9">
       <c r="C96" s="1">
-        <v>1291700</v>
+        <v>1291800</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -5388,7 +5388,7 @@
     </row>
     <row r="100" spans="3:9">
       <c r="C100" s="1">
-        <v>1181200</v>
+        <v>1181100</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -5411,7 +5411,7 @@
     </row>
     <row r="101" spans="3:9">
       <c r="C101" s="1">
-        <v>1150800</v>
+        <v>1150700</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -5434,7 +5434,7 @@
     </row>
     <row r="102" spans="3:9">
       <c r="C102" s="1">
-        <v>1119200</v>
+        <v>1119000</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -5457,7 +5457,7 @@
     </row>
     <row r="103" spans="3:9">
       <c r="C103" s="1">
-        <v>1086200</v>
+        <v>1086000</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -5480,7 +5480,7 @@
     </row>
     <row r="104" spans="3:9">
       <c r="C104" s="1">
-        <v>1051900</v>
+        <v>1051600</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -5510,7 +5510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:I104"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -7878,8 +7878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:D102"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8697,7 +8697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:D102"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>